<commit_message>
Latest Update - Hate Crime
Added Hate Crime as a measure
</commit_message>
<xml_diff>
--- a/State_Of_London_Crime.xlsx
+++ b/State_Of_London_Crime.xlsx
@@ -16,12 +16,13 @@
     <sheet name="Burglary_Offences" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="TfMV_Offences" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Theft_Person" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Hate_Crime" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Month_Year</t>
   </si>
@@ -62,6 +63,12 @@
     <t xml:space="preserve">Rape</t>
   </si>
   <si>
+    <t xml:space="preserve">Sexual Offences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of offences recorded by the MPS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Non-Domestic Knife Crime with Injury Offences – Victim U25</t>
   </si>
   <si>
@@ -92,10 +99,13 @@
     <t xml:space="preserve">Number of offences recorded by the MPS (Thousands)</t>
   </si>
   <si>
-    <t xml:space="preserve">Sexual Offences</t>
+    <t xml:space="preserve">metal</t>
   </si>
   <si>
-    <t xml:space="preserve">The number of offences recorded by the MPS</t>
+    <t xml:space="preserve">Hate Crime Offences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of hate crime offences in London as recorded by the MPS</t>
   </si>
 </sst>
 </file>
@@ -1068,7 +1078,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -1082,7 +1092,7 @@
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -1619,6 +1629,606 @@
       </c>
       <c r="B71" t="n">
         <v>6934</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>42826</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1610</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>42856</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1705</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>42887</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2149</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>42917</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>42948</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>42979</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>43009</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>43040</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>43070</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>43101</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>43132</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>43160</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>43191</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>43221</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>43252</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>43282</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>43313</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>43344</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>43374</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>43405</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>43435</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>43466</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>43497</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>43525</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>43556</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>43586</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>43617</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>43647</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>43678</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>43709</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>43739</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>43770</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>43800</v>
+      </c>
+      <c r="B34" t="n">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>43831</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>43862</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>43891</v>
+      </c>
+      <c r="B37" t="n">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>43922</v>
+      </c>
+      <c r="B38" t="n">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>43952</v>
+      </c>
+      <c r="B39" t="n">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>43983</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>44013</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2710</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>44044</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>44075</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>44105</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>44136</v>
+      </c>
+      <c r="B45" t="n">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44166</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>44197</v>
+      </c>
+      <c r="B47" t="n">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>44228</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B49" t="n">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>44287</v>
+      </c>
+      <c r="B50" t="n">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>44317</v>
+      </c>
+      <c r="B51" t="n">
+        <v>2573</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B52" t="n">
+        <v>2537</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>44378</v>
+      </c>
+      <c r="B53" t="n">
+        <v>2810</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>44409</v>
+      </c>
+      <c r="B54" t="n">
+        <v>2219</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>44440</v>
+      </c>
+      <c r="B55" t="n">
+        <v>2188</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>44470</v>
+      </c>
+      <c r="B56" t="n">
+        <v>2310</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>44501</v>
+      </c>
+      <c r="B57" t="n">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>44531</v>
+      </c>
+      <c r="B58" t="n">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>44562</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>44593</v>
+      </c>
+      <c r="B60" t="n">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>44621</v>
+      </c>
+      <c r="B61" t="n">
+        <v>2227</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B65" t="n">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B66" t="n">
+        <v>2242</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B67" t="n">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B68" t="n">
+        <v>2876</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B69" t="n">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B70" t="n">
+        <v>2281</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>45292</v>
+      </c>
+      <c r="B71" t="n">
+        <v>2042</v>
       </c>
     </row>
   </sheetData>
@@ -2877,7 +3487,7 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -2894,7 +3504,7 @@
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -3681,7 +4291,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -4281,7 +4891,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -4295,7 +4905,7 @@
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -4881,7 +5491,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -5453,10 +6063,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -5490,7 +6100,7 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
@@ -6294,7 +6904,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Added missing financial year for both TNO and Other data
Accidentally omitted the 22/23 financial year from the SoL report. Have now included the missing year so report runs from 2017 - 2024 (January)
</commit_message>
<xml_diff>
--- a/State_Of_London_Crime.xlsx
+++ b/State_Of_London_Crime.xlsx
@@ -953,81 +953,177 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45017</v>
+        <v>44652</v>
       </c>
       <c r="B62" t="n">
-        <v>80706</v>
+        <v>77220</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45047</v>
+        <v>44682</v>
       </c>
       <c r="B63" t="n">
-        <v>87619</v>
+        <v>84965</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45078</v>
+        <v>44713</v>
       </c>
       <c r="B64" t="n">
-        <v>90899</v>
+        <v>82257</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45108</v>
+        <v>44743</v>
       </c>
       <c r="B65" t="n">
-        <v>89858</v>
+        <v>84417</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45139</v>
+        <v>44774</v>
       </c>
       <c r="B66" t="n">
-        <v>85707</v>
+        <v>82536</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45170</v>
+        <v>44805</v>
       </c>
       <c r="B67" t="n">
-        <v>86695</v>
+        <v>77936</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45200</v>
+        <v>44835</v>
       </c>
       <c r="B68" t="n">
-        <v>91638</v>
+        <v>85312</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45231</v>
+        <v>44866</v>
       </c>
       <c r="B69" t="n">
-        <v>88188</v>
+        <v>84552</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45261</v>
+        <v>44896</v>
       </c>
       <c r="B70" t="n">
-        <v>86651</v>
+        <v>78288</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B71" t="n">
+        <v>82652</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B72" t="n">
+        <v>77739</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B73" t="n">
+        <v>86703</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B74" t="n">
+        <v>80706</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B75" t="n">
+        <v>87619</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B76" t="n">
+        <v>90899</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B77" t="n">
+        <v>89858</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B78" t="n">
+        <v>85707</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B79" t="n">
+        <v>86695</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B80" t="n">
+        <v>91638</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B81" t="n">
+        <v>88188</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B82" t="n">
+        <v>86651</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
         <v>45292</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B83" t="n">
         <v>84229</v>
       </c>
     </row>
@@ -1553,81 +1649,177 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45017</v>
+        <v>44652</v>
       </c>
       <c r="B62" t="n">
-        <v>5647</v>
+        <v>4568</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45047</v>
+        <v>44682</v>
       </c>
       <c r="B63" t="n">
-        <v>5675</v>
+        <v>4737</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45078</v>
+        <v>44713</v>
       </c>
       <c r="B64" t="n">
-        <v>5517</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45108</v>
+        <v>44743</v>
       </c>
       <c r="B65" t="n">
-        <v>5491</v>
+        <v>4920</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45139</v>
+        <v>44774</v>
       </c>
       <c r="B66" t="n">
-        <v>5038</v>
+        <v>3853</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45170</v>
+        <v>44805</v>
       </c>
       <c r="B67" t="n">
-        <v>5006</v>
+        <v>3589</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45200</v>
+        <v>44835</v>
       </c>
       <c r="B68" t="n">
-        <v>6668</v>
+        <v>5603</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45231</v>
+        <v>44866</v>
       </c>
       <c r="B69" t="n">
-        <v>8458</v>
+        <v>6039</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45261</v>
+        <v>44896</v>
       </c>
       <c r="B70" t="n">
-        <v>8182</v>
+        <v>6111</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B71" t="n">
+        <v>5567</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B72" t="n">
+        <v>5572</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B73" t="n">
+        <v>5896</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B74" t="n">
+        <v>5647</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B75" t="n">
+        <v>5675</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B76" t="n">
+        <v>5517</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B77" t="n">
+        <v>5491</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B78" t="n">
+        <v>5038</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B79" t="n">
+        <v>5006</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B80" t="n">
+        <v>6668</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B81" t="n">
+        <v>8458</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B82" t="n">
+        <v>8182</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
         <v>45292</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B83" t="n">
         <v>6934</v>
       </c>
     </row>
@@ -2153,81 +2345,177 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45017</v>
+        <v>44652</v>
       </c>
       <c r="B62" t="n">
-        <v>2002</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45047</v>
+        <v>44682</v>
       </c>
       <c r="B63" t="n">
-        <v>2305</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45078</v>
+        <v>44713</v>
       </c>
       <c r="B64" t="n">
-        <v>2425</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45108</v>
+        <v>44743</v>
       </c>
       <c r="B65" t="n">
-        <v>2330</v>
+        <v>2354</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45139</v>
+        <v>44774</v>
       </c>
       <c r="B66" t="n">
-        <v>2242</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45170</v>
+        <v>44805</v>
       </c>
       <c r="B67" t="n">
-        <v>2305</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45200</v>
+        <v>44835</v>
       </c>
       <c r="B68" t="n">
-        <v>2876</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45231</v>
+        <v>44866</v>
       </c>
       <c r="B69" t="n">
-        <v>2705</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45261</v>
+        <v>44896</v>
       </c>
       <c r="B70" t="n">
-        <v>2281</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B73" t="n">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B76" t="n">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B77" t="n">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B78" t="n">
+        <v>2242</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B79" t="n">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B80" t="n">
+        <v>2876</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B81" t="n">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B82" t="n">
+        <v>2281</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
         <v>45292</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B83" t="n">
         <v>2042</v>
       </c>
     </row>
@@ -2753,81 +3041,177 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45017</v>
+        <v>44652</v>
       </c>
       <c r="B62" t="n">
-        <v>6337</v>
+        <v>6170</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45047</v>
+        <v>44682</v>
       </c>
       <c r="B63" t="n">
-        <v>7155</v>
+        <v>7019</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45078</v>
+        <v>44713</v>
       </c>
       <c r="B64" t="n">
-        <v>7736</v>
+        <v>6855</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45108</v>
+        <v>44743</v>
       </c>
       <c r="B65" t="n">
-        <v>7279</v>
+        <v>7243</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45139</v>
+        <v>44774</v>
       </c>
       <c r="B66" t="n">
-        <v>6822</v>
+        <v>6807</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45170</v>
+        <v>44805</v>
       </c>
       <c r="B67" t="n">
-        <v>7057</v>
+        <v>6415</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45200</v>
+        <v>44835</v>
       </c>
       <c r="B68" t="n">
-        <v>6780</v>
+        <v>6725</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45231</v>
+        <v>44866</v>
       </c>
       <c r="B69" t="n">
-        <v>6322</v>
+        <v>6334</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45261</v>
+        <v>44896</v>
       </c>
       <c r="B70" t="n">
-        <v>6732</v>
+        <v>5926</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B71" t="n">
+        <v>5889</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B72" t="n">
+        <v>5728</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B73" t="n">
+        <v>6349</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B74" t="n">
+        <v>6337</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B75" t="n">
+        <v>7155</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B76" t="n">
+        <v>7736</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B77" t="n">
+        <v>7279</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B78" t="n">
+        <v>6822</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B79" t="n">
+        <v>7057</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B80" t="n">
+        <v>6780</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B81" t="n">
+        <v>6322</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B82" t="n">
+        <v>6732</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
         <v>45292</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B83" t="n">
         <v>6100</v>
       </c>
     </row>
@@ -3353,81 +3737,177 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45017</v>
+        <v>44652</v>
       </c>
       <c r="B62" t="n">
-        <v>8133</v>
+        <v>7711</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45047</v>
+        <v>44682</v>
       </c>
       <c r="B63" t="n">
-        <v>8378</v>
+        <v>8251</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45078</v>
+        <v>44713</v>
       </c>
       <c r="B64" t="n">
-        <v>8770</v>
+        <v>7936</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45108</v>
+        <v>44743</v>
       </c>
       <c r="B65" t="n">
-        <v>8581</v>
+        <v>8529</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45139</v>
+        <v>44774</v>
       </c>
       <c r="B66" t="n">
-        <v>8173</v>
+        <v>8419</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45170</v>
+        <v>44805</v>
       </c>
       <c r="B67" t="n">
-        <v>8145</v>
+        <v>7732</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45200</v>
+        <v>44835</v>
       </c>
       <c r="B68" t="n">
-        <v>7995</v>
+        <v>8098</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45231</v>
+        <v>44866</v>
       </c>
       <c r="B69" t="n">
-        <v>7287</v>
+        <v>7610</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45261</v>
+        <v>44896</v>
       </c>
       <c r="B70" t="n">
-        <v>8024</v>
+        <v>7839</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B71" t="n">
+        <v>8027</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B72" t="n">
+        <v>7201</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B73" t="n">
+        <v>8031</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B74" t="n">
+        <v>8133</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B75" t="n">
+        <v>8378</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B76" t="n">
+        <v>8770</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B77" t="n">
+        <v>8581</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B78" t="n">
+        <v>8173</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B79" t="n">
+        <v>8145</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B80" t="n">
+        <v>7995</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B81" t="n">
+        <v>7287</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B82" t="n">
+        <v>8024</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
         <v>45292</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B83" t="n">
         <v>7627</v>
       </c>
     </row>
@@ -4136,111 +4616,243 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45017</v>
+        <v>44652</v>
       </c>
       <c r="B62" t="n">
-        <v>1164</v>
+        <v>1209</v>
       </c>
       <c r="C62" t="n">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45047</v>
+        <v>44682</v>
       </c>
       <c r="B63" t="n">
-        <v>1447</v>
+        <v>1496</v>
       </c>
       <c r="C63" t="n">
-        <v>785</v>
+        <v>823</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45078</v>
+        <v>44713</v>
       </c>
       <c r="B64" t="n">
-        <v>1472</v>
+        <v>1421</v>
       </c>
       <c r="C64" t="n">
-        <v>723</v>
+        <v>751</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45108</v>
+        <v>44743</v>
       </c>
       <c r="B65" t="n">
-        <v>1409</v>
+        <v>1551</v>
       </c>
       <c r="C65" t="n">
-        <v>752</v>
+        <v>797</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45139</v>
+        <v>44774</v>
       </c>
       <c r="B66" t="n">
-        <v>1255</v>
+        <v>1367</v>
       </c>
       <c r="C66" t="n">
-        <v>723</v>
+        <v>754</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45170</v>
+        <v>44805</v>
       </c>
       <c r="B67" t="n">
-        <v>1422</v>
+        <v>1298</v>
       </c>
       <c r="C67" t="n">
-        <v>766</v>
+        <v>757</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45200</v>
+        <v>44835</v>
       </c>
       <c r="B68" t="n">
-        <v>1309</v>
+        <v>1360</v>
       </c>
       <c r="C68" t="n">
-        <v>757</v>
+        <v>779</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45231</v>
+        <v>44866</v>
       </c>
       <c r="B69" t="n">
-        <v>1232</v>
+        <v>1360</v>
       </c>
       <c r="C69" t="n">
-        <v>664</v>
+        <v>755</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45261</v>
+        <v>44896</v>
       </c>
       <c r="B70" t="n">
-        <v>1177</v>
+        <v>1031</v>
       </c>
       <c r="C70" t="n">
-        <v>666</v>
+        <v>681</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1202</v>
+      </c>
+      <c r="C71" t="n">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1151</v>
+      </c>
+      <c r="C72" t="n">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B73" t="n">
+        <v>1369</v>
+      </c>
+      <c r="C73" t="n">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B74" t="n">
+        <v>1164</v>
+      </c>
+      <c r="C74" t="n">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B75" t="n">
+        <v>1447</v>
+      </c>
+      <c r="C75" t="n">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B76" t="n">
+        <v>1472</v>
+      </c>
+      <c r="C76" t="n">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B77" t="n">
+        <v>1409</v>
+      </c>
+      <c r="C77" t="n">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B78" t="n">
+        <v>1255</v>
+      </c>
+      <c r="C78" t="n">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B79" t="n">
+        <v>1422</v>
+      </c>
+      <c r="C79" t="n">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B80" t="n">
+        <v>1309</v>
+      </c>
+      <c r="C80" t="n">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B81" t="n">
+        <v>1232</v>
+      </c>
+      <c r="C81" t="n">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B82" t="n">
+        <v>1177</v>
+      </c>
+      <c r="C82" t="n">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
         <v>45292</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B83" t="n">
         <v>1143</v>
       </c>
-      <c r="C71" t="n">
+      <c r="C83" t="n">
         <v>696</v>
       </c>
     </row>
@@ -4766,81 +5378,177 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45017</v>
+        <v>44652</v>
       </c>
       <c r="B62" t="n">
-        <v>115</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45047</v>
+        <v>44682</v>
       </c>
       <c r="B63" t="n">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45078</v>
+        <v>44713</v>
       </c>
       <c r="B64" t="n">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45108</v>
+        <v>44743</v>
       </c>
       <c r="B65" t="n">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45139</v>
+        <v>44774</v>
       </c>
       <c r="B66" t="n">
-        <v>122</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45170</v>
+        <v>44805</v>
       </c>
       <c r="B67" t="n">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45200</v>
+        <v>44835</v>
       </c>
       <c r="B68" t="n">
-        <v>92</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45231</v>
+        <v>44866</v>
       </c>
       <c r="B69" t="n">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45261</v>
+        <v>44896</v>
       </c>
       <c r="B70" t="n">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B71" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B72" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B73" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B74" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B75" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B76" t="n">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B77" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B78" t="n">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B79" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B80" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B81" t="n">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B82" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
         <v>45292</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B83" t="n">
         <v>97</v>
       </c>
     </row>
@@ -5366,81 +6074,177 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45017</v>
+        <v>44652</v>
       </c>
       <c r="B62" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45047</v>
+        <v>44682</v>
       </c>
       <c r="B63" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45078</v>
+        <v>44713</v>
       </c>
       <c r="B64" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45108</v>
+        <v>44743</v>
       </c>
       <c r="B65" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45139</v>
+        <v>44774</v>
       </c>
       <c r="B66" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45170</v>
+        <v>44805</v>
       </c>
       <c r="B67" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45200</v>
+        <v>44835</v>
       </c>
       <c r="B68" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45231</v>
+        <v>44866</v>
       </c>
       <c r="B69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45261</v>
+        <v>44896</v>
       </c>
       <c r="B70" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B71" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B72" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B73" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B74" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B75" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B76" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B77" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B78" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B79" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B80" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B81" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B82" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
         <v>45292</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B83" t="n">
         <v>9</v>
       </c>
     </row>
@@ -5966,81 +6770,177 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45017</v>
+        <v>44652</v>
       </c>
       <c r="B62" t="n">
-        <v>2295</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45047</v>
+        <v>44682</v>
       </c>
       <c r="B63" t="n">
-        <v>2567</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45078</v>
+        <v>44713</v>
       </c>
       <c r="B64" t="n">
-        <v>2531</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45108</v>
+        <v>44743</v>
       </c>
       <c r="B65" t="n">
-        <v>2442</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45139</v>
+        <v>44774</v>
       </c>
       <c r="B66" t="n">
-        <v>2218</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45170</v>
+        <v>44805</v>
       </c>
       <c r="B67" t="n">
-        <v>2473</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45200</v>
+        <v>44835</v>
       </c>
       <c r="B68" t="n">
-        <v>2535</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45231</v>
+        <v>44866</v>
       </c>
       <c r="B69" t="n">
-        <v>2691</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45261</v>
+        <v>44896</v>
       </c>
       <c r="B70" t="n">
-        <v>2799</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B71" t="n">
+        <v>2398</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B72" t="n">
+        <v>2457</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B73" t="n">
+        <v>2429</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2295</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2567</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B76" t="n">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B77" t="n">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B78" t="n">
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B79" t="n">
+        <v>2473</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B80" t="n">
+        <v>2535</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B81" t="n">
+        <v>2691</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B82" t="n">
+        <v>2799</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
         <v>45292</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B83" t="n">
         <v>2577</v>
       </c>
     </row>
@@ -6749,111 +7649,243 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45017</v>
+        <v>44652</v>
       </c>
       <c r="B62" t="n">
-        <v>2992</v>
+        <v>2846</v>
       </c>
       <c r="C62" t="n">
-        <v>1538</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45047</v>
+        <v>44682</v>
       </c>
       <c r="B63" t="n">
-        <v>2941</v>
+        <v>3210</v>
       </c>
       <c r="C63" t="n">
-        <v>1623</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45078</v>
+        <v>44713</v>
       </c>
       <c r="B64" t="n">
-        <v>2971</v>
+        <v>2904</v>
       </c>
       <c r="C64" t="n">
-        <v>1476</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45108</v>
+        <v>44743</v>
       </c>
       <c r="B65" t="n">
-        <v>3167</v>
+        <v>2648</v>
       </c>
       <c r="C65" t="n">
-        <v>1418</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45139</v>
+        <v>44774</v>
       </c>
       <c r="B66" t="n">
-        <v>3288</v>
+        <v>2898</v>
       </c>
       <c r="C66" t="n">
-        <v>1483</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45170</v>
+        <v>44805</v>
       </c>
       <c r="B67" t="n">
-        <v>3185</v>
+        <v>3165</v>
       </c>
       <c r="C67" t="n">
-        <v>1467</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45200</v>
+        <v>44835</v>
       </c>
       <c r="B68" t="n">
-        <v>3280</v>
+        <v>3359</v>
       </c>
       <c r="C68" t="n">
-        <v>1574</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45231</v>
+        <v>44866</v>
       </c>
       <c r="B69" t="n">
-        <v>3316</v>
+        <v>3465</v>
       </c>
       <c r="C69" t="n">
-        <v>1382</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45261</v>
+        <v>44896</v>
       </c>
       <c r="B70" t="n">
-        <v>3513</v>
+        <v>3233</v>
       </c>
       <c r="C70" t="n">
-        <v>1502</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B71" t="n">
+        <v>3463</v>
+      </c>
+      <c r="C71" t="n">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B72" t="n">
+        <v>3049</v>
+      </c>
+      <c r="C72" t="n">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B73" t="n">
+        <v>3252</v>
+      </c>
+      <c r="C73" t="n">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2992</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2941</v>
+      </c>
+      <c r="C75" t="n">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B76" t="n">
+        <v>2971</v>
+      </c>
+      <c r="C76" t="n">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B77" t="n">
+        <v>3167</v>
+      </c>
+      <c r="C77" t="n">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B78" t="n">
+        <v>3288</v>
+      </c>
+      <c r="C78" t="n">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B79" t="n">
+        <v>3185</v>
+      </c>
+      <c r="C79" t="n">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B80" t="n">
+        <v>3280</v>
+      </c>
+      <c r="C80" t="n">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B81" t="n">
+        <v>3316</v>
+      </c>
+      <c r="C81" t="n">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B82" t="n">
+        <v>3513</v>
+      </c>
+      <c r="C82" t="n">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
         <v>45292</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B83" t="n">
         <v>3575</v>
       </c>
-      <c r="C71" t="n">
+      <c r="C83" t="n">
         <v>1508</v>
       </c>
     </row>
@@ -7379,81 +8411,177 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45017</v>
+        <v>44652</v>
       </c>
       <c r="B62" t="n">
-        <v>4652</v>
+        <v>5152</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45047</v>
+        <v>44682</v>
       </c>
       <c r="B63" t="n">
-        <v>5001</v>
+        <v>5177</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45078</v>
+        <v>44713</v>
       </c>
       <c r="B64" t="n">
-        <v>4850</v>
+        <v>5376</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45108</v>
+        <v>44743</v>
       </c>
       <c r="B65" t="n">
-        <v>4824</v>
+        <v>5328</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45139</v>
+        <v>44774</v>
       </c>
       <c r="B66" t="n">
-        <v>4818</v>
+        <v>5457</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45170</v>
+        <v>44805</v>
       </c>
       <c r="B67" t="n">
-        <v>5012</v>
+        <v>5767</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45200</v>
+        <v>44835</v>
       </c>
       <c r="B68" t="n">
-        <v>5833</v>
+        <v>6079</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45231</v>
+        <v>44866</v>
       </c>
       <c r="B69" t="n">
-        <v>5112</v>
+        <v>5825</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45261</v>
+        <v>44896</v>
       </c>
       <c r="B70" t="n">
-        <v>4897</v>
+        <v>4784</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B71" t="n">
+        <v>5420</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B72" t="n">
+        <v>4974</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B73" t="n">
+        <v>5503</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>45017</v>
+      </c>
+      <c r="B74" t="n">
+        <v>4652</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B75" t="n">
+        <v>5001</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B76" t="n">
+        <v>4850</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B77" t="n">
+        <v>4824</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B78" t="n">
+        <v>4818</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B79" t="n">
+        <v>5012</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B80" t="n">
+        <v>5833</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B81" t="n">
+        <v>5112</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B82" t="n">
+        <v>4897</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
         <v>45292</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B83" t="n">
         <v>4998</v>
       </c>
     </row>

</xml_diff>